<commit_message>
Cap nhat noi dung
</commit_message>
<xml_diff>
--- a/MyMmoIdea.xlsx
+++ b/MyMmoIdea.xlsx
@@ -18,15 +18,106 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+  <si>
+    <t>Ý Tưởng MMO 2019</t>
+  </si>
+  <si>
+    <t>Xây dựng kênh download</t>
+  </si>
+  <si>
+    <t>Xây dựng hệ thông MMO qua link rút gọn</t>
+  </si>
+  <si>
+    <t>Xây dựng các kênh truyền tải nội dung để hướng người dùng download nội dung đó</t>
+  </si>
+  <si>
+    <t>Từ đấy thông qua hệ thống link rút gọn để kiếm $ từ việc người dùng click vào link download</t>
+  </si>
+  <si>
+    <t>Các hình thức</t>
+  </si>
+  <si>
+    <t>Xây dựng website</t>
+  </si>
+  <si>
+    <t>Xây dựng kênh youtube và các kênh tạo video khác</t>
+  </si>
+  <si>
+    <t>Chạy trực tiếp quảng cáo</t>
+  </si>
+  <si>
+    <t>Hạn chế các nội dung vi phạm bản quyền lớn vì dễ bị kiện</t>
+  </si>
+  <si>
+    <t>Nên tập trung các nội dung không vi phạm bản quyền, các nội dung quảng bá free cho các kênh thương hiệu mới</t>
+  </si>
+  <si>
+    <t>Đi link trên các diễn đàn</t>
+  </si>
+  <si>
+    <t>Xây dựng hệ thống đối tượng hướng đến, theo các chủ đề khác nhau thì hướng đến đối tượng khác nhau</t>
+  </si>
+  <si>
+    <t>Ăn theo trend</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Các chủ đề download</t>
+  </si>
+  <si>
+    <t>Nhạc mp3</t>
+  </si>
+  <si>
+    <t>Tài liệu</t>
+  </si>
+  <si>
+    <t>Ứng dụng</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Torrent link</t>
+  </si>
+  <si>
+    <t>Nội dung các chủ đề</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +425,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>